<commit_message>
renamed some variables for clarity separated pro(pro-com creation method into two separate methods
</commit_message>
<xml_diff>
--- a/gui/IDP_MapTool_Flask/pandapower2urbs/dataset/_transmission/test.xlsx
+++ b/gui/IDP_MapTool_Flask/pandapower2urbs/dataset/_transmission/test.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="193">
   <si>
     <t>name</t>
   </si>
@@ -495,18 +495,18 @@
     <t>0.63 MVA 10/0.4 kV</t>
   </si>
   <si>
+    <t>sn_hv_mva</t>
+  </si>
+  <si>
+    <t>sn_mv_mva</t>
+  </si>
+  <si>
+    <t>sn_lv_mva</t>
+  </si>
+  <si>
     <t>vn_mv_kv</t>
   </si>
   <si>
-    <t>sn_hv_mva</t>
-  </si>
-  <si>
-    <t>sn_mv_mva</t>
-  </si>
-  <si>
-    <t>sn_lv_mva</t>
-  </si>
-  <si>
     <t>vk_hv_percent</t>
   </si>
   <si>
@@ -531,10 +531,16 @@
     <t>shift_lv_degree</t>
   </si>
   <si>
+    <t>vector_group</t>
+  </si>
+  <si>
     <t>63/25/38 MVA 110/20/10 kV</t>
   </si>
   <si>
     <t>63/25/38 MVA 110/10/10 kV</t>
+  </si>
+  <si>
+    <t>YN0yn0yn0</t>
   </si>
   <si>
     <t>element</t>
@@ -1129,30 +1135,30 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>160</v>
@@ -1185,42 +1191,45 @@
         <v>167</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B2">
+        <v>63</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>38</v>
+      </c>
+      <c r="E2">
         <v>110</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>10</v>
-      </c>
-      <c r="E2">
-        <v>63</v>
-      </c>
-      <c r="F2">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>38</v>
       </c>
       <c r="H2">
         <v>10.4</v>
@@ -1253,42 +1262,45 @@
         <v>0</v>
       </c>
       <c r="R2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" t="s">
         <v>75</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
       <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>-10</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>10</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>38</v>
+      </c>
+      <c r="E3">
         <v>110</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="G3">
         <v>10</v>
-      </c>
-      <c r="E3">
-        <v>63</v>
-      </c>
-      <c r="F3">
-        <v>25</v>
-      </c>
-      <c r="G3">
-        <v>38</v>
       </c>
       <c r="H3">
         <v>10.4</v>
@@ -1321,18 +1333,21 @@
         <v>0</v>
       </c>
       <c r="R3" t="s">
+        <v>171</v>
+      </c>
+      <c r="S3" t="s">
         <v>75</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
       <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>-10</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>10</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>1.2</v>
       </c>
     </row>
@@ -1351,13 +1366,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1371,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1385,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1399,7 +1414,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1413,7 +1428,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1427,7 +1442,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1441,7 +1456,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1455,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1463,13 +1478,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1477,13 +1492,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1491,13 +1506,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1505,13 +1520,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1519,13 +1534,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1533,13 +1548,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1547,13 +1562,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1561,13 +1576,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1575,13 +1590,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1589,13 +1604,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1603,13 +1618,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1617,13 +1632,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1631,13 +1646,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1645,13 +1660,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C22" t="s">
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1659,13 +1674,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1673,13 +1688,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1687,13 +1702,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1701,13 +1716,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1715,13 +1730,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1729,13 +1744,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
         <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1743,13 +1758,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1757,13 +1772,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
         <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1771,13 +1786,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1785,13 +1800,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1799,13 +1814,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1813,13 +1828,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1827,13 +1842,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1841,13 +1856,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1855,13 +1870,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1869,13 +1884,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C38" t="s">
         <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1883,13 +1898,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1897,13 +1912,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
         <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1911,13 +1926,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1925,13 +1940,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1939,13 +1954,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C43" t="s">
         <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1953,13 +1968,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C44" t="s">
         <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1967,13 +1982,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
         <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1981,13 +1996,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1995,13 +2010,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C47" t="s">
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2009,13 +2024,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
         <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2023,13 +2038,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2037,13 +2052,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s">
         <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2051,13 +2066,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C51" t="s">
         <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2065,13 +2080,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C52" t="s">
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2079,13 +2094,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2093,13 +2108,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C54" t="s">
         <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2107,13 +2122,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C55" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2121,13 +2136,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2135,13 +2150,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C57" t="s">
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2149,13 +2164,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2163,13 +2178,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2177,13 +2192,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
         <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2191,13 +2206,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C61" t="s">
         <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2205,13 +2220,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C62" t="s">
         <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2219,13 +2234,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C63" t="s">
         <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2233,13 +2248,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C64" t="s">
         <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2247,13 +2262,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
         <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2261,13 +2276,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C66" t="s">
         <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2275,13 +2290,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C67" t="s">
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2289,13 +2304,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C68" t="s">
         <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2303,13 +2318,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C69" t="s">
         <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2317,13 +2332,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C70" t="s">
         <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2331,13 +2346,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C71" t="s">
         <v>68</v>
       </c>
       <c r="D71" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2345,13 +2360,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C72" t="s">
         <v>69</v>
       </c>
       <c r="D72" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2359,13 +2374,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C73" t="s">
         <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2373,13 +2388,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C74" t="s">
         <v>71</v>
       </c>
       <c r="D74" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2387,13 +2402,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C75" t="s">
         <v>49</v>
       </c>
       <c r="D75" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2401,13 +2416,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C76" t="s">
         <v>48</v>
       </c>
       <c r="D76" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2415,13 +2430,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C77" t="s">
         <v>4</v>
       </c>
       <c r="D77" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2429,13 +2444,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C78" t="s">
         <v>72</v>
       </c>
       <c r="D78" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2443,13 +2458,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C79" t="s">
         <v>82</v>
       </c>
       <c r="D79" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2457,13 +2472,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C80" t="s">
         <v>80</v>
       </c>
       <c r="D80" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2471,13 +2486,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C81" t="s">
         <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2485,13 +2500,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C82" t="s">
         <v>82</v>
       </c>
       <c r="D82" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2509,22 +2524,22 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>19</v>
@@ -2535,10 +2550,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>

</xml_diff>